<commit_message>
Created excel file to work on data locally
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="149">
   <si>
     <t>7360 TEST 38 ST</t>
   </si>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="BH1" sqref="BH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,6 +807,9 @@
     <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="24" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="29" bestFit="1" customWidth="1"/>
@@ -1611,9 +1614,6 @@
       <c r="D4" t="s">
         <v>143</v>
       </c>
-      <c r="E4" t="s">
-        <v>124</v>
-      </c>
       <c r="F4">
         <v>92103</v>
       </c>

</xml_diff>